<commit_message>
Replace input data for energy supplier cash flow entities with internal calculations or assignment (#135)
</commit_message>
<xml_diff>
--- a/InputData/bldgs/FoBObE/Frac of Bldgs Owned by Entity.xlsx
+++ b/InputData/bldgs/FoBObE/Frac of Bldgs Owned by Entity.xlsx
@@ -1,37 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\FoBObE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\bldgs\FoBObE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D1B2A-0F82-4946-A7E8-65637F63812F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="23955" windowHeight="12840"/>
+    <workbookView xWindow="16455" yWindow="150" windowWidth="29520" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Residential" sheetId="2" r:id="rId2"/>
     <sheet name="Commercial" sheetId="3" r:id="rId3"/>
-    <sheet name="Output by Industry" sheetId="5" r:id="rId4"/>
-    <sheet name="FoBObE" sheetId="4" r:id="rId5"/>
+    <sheet name="FoBObE" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="outputfrac_bio">'Output by Industry'!$A$9</definedName>
-    <definedName name="outputfrac_coal">'Output by Industry'!$A$7</definedName>
-    <definedName name="outputfrac_elec">'Output by Industry'!$A$6</definedName>
-    <definedName name="outputfrac_ngps">'Output by Industry'!$A$8</definedName>
-    <definedName name="outputfrac_nonenergy">'Output by Industry'!$A$5</definedName>
-    <definedName name="outputfrac_other">'Output by Industry'!$A$10</definedName>
+    <definedName name="outputfrac_bio">#REF!</definedName>
+    <definedName name="outputfrac_coal">#REF!</definedName>
+    <definedName name="outputfrac_elec">#REF!</definedName>
+    <definedName name="outputfrac_ngps">#REF!</definedName>
+    <definedName name="outputfrac_nonenergy">#REF!</definedName>
+    <definedName name="outputfrac_other">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>Sources:</t>
   </si>
@@ -213,60 +224,12 @@
     <t>foreign entities</t>
   </si>
   <si>
-    <t>nonenergy industries</t>
-  </si>
-  <si>
     <t>labor and consumers</t>
   </si>
   <si>
-    <t>electricity suppliers</t>
-  </si>
-  <si>
-    <t>coal suppliers</t>
-  </si>
-  <si>
-    <t>natural gas and petroleum suppliers</t>
-  </si>
-  <si>
-    <t>biomass and biofuel suppliers</t>
-  </si>
-  <si>
-    <t>other energy suppliers</t>
-  </si>
-  <si>
-    <t>For bibliographic source and methods, see file output_shares_by_industry.xslx</t>
-  </si>
-  <si>
-    <t>in the InputData folder.</t>
-  </si>
-  <si>
-    <t>Share</t>
-  </si>
-  <si>
-    <t>Industry Category</t>
-  </si>
-  <si>
-    <t>non-energy industries</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>For commercial buildings, we divde between "nonenergy industries" and</t>
-  </si>
-  <si>
-    <t>the various energy industries based on output shares of GDP.  (We assume</t>
-  </si>
-  <si>
-    <t>that all residential buildings owned by industry are owned by "nonenergy</t>
-  </si>
-  <si>
-    <t>industries" - i.e. rental property management communities, nursing homes,</t>
-  </si>
-  <si>
-    <t>etc. - not energy industries.</t>
-  </si>
-  <si>
     <t>In the output tab, we show more decimal places than the source data</t>
   </si>
   <si>
@@ -276,24 +239,23 @@
     <t>provide in order to avoid rounding error in Vensim (each column must</t>
   </si>
   <si>
-    <t>Fraction of buildings owned by cash flow entity is used in cash flow calculations.</t>
-  </si>
-  <si>
     <t>Ownership by Cash Flow Entity (dimensionless)</t>
+  </si>
+  <si>
+    <t>domestic industries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +318,14 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -541,7 +511,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -648,7 +618,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -685,8 +654,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -785,6 +753,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -820,6 +805,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -995,12 +997,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1077,60 +1077,30 @@
         <v>7</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>72</v>
+      <c r="A18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
-        <v>81</v>
+      <c r="A19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -1138,7 +1108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1158,20 +1128,20 @@
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -1199,60 +1169,60 @@
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="64" t="s">
+      <c r="K5" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="65" t="s">
+      <c r="O5" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="66"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="65"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
       <c r="F6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="67" t="s">
+      <c r="K6" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
       <c r="N6" s="14"/>
-      <c r="O6" s="67" t="s">
+      <c r="O6" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="68"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="67"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -1414,85 +1384,85 @@
       <c r="A13" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="60"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="59"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="60"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="59"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="60"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="59"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="62"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="61"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1638,7 +1608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1973,24 +1943,24 @@
       <c r="A16" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-      <c r="Q16" s="70"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="69"/>
     </row>
     <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -2036,94 +2006,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="56">
-        <v>0.93219819361870848</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
-        <v>1.5490855293616566E-2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="56">
-        <v>2.1866536828369144E-3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="56">
-        <v>4.9443136381930888E-2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
-        <v>6.8116102290716575E-4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2136,8 +2023,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
-        <v>82</v>
+      <c r="A1" s="70" t="s">
+        <v>65</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>57</v>
@@ -2153,45 +2040,45 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="57">
         <f>Residential!C34</f>
         <v>1.9289972368294446E-2</v>
       </c>
-      <c r="C2" s="58">
+      <c r="C2" s="57">
         <f>B2</f>
         <v>1.9289972368294446E-2</v>
       </c>
-      <c r="D2" s="58">
+      <c r="D2" s="57">
         <f>Commercial!C20</f>
         <v>0.23714188688565077</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="58">
+        <v>66</v>
+      </c>
+      <c r="B3" s="57">
         <f>Residential!C35</f>
         <v>3.6530988312536733E-2</v>
       </c>
-      <c r="C3" s="58">
-        <f t="shared" ref="C3:C10" si="0">B3</f>
+      <c r="C3" s="57">
+        <f t="shared" ref="C3:C5" si="0">B3</f>
         <v>3.6530988312536733E-2</v>
       </c>
-      <c r="D3" s="58">
-        <f>Commercial!$C$21*outputfrac_nonenergy</f>
-        <v>0.71113495503257274</v>
+      <c r="D3" s="57">
+        <f>Commercial!$C$21</f>
+        <v>0.76285811311434926</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="58">
+        <v>60</v>
+      </c>
+      <c r="B4" s="57">
         <f>Residential!C36</f>
         <v>0.94417903931916869</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="57">
         <f t="shared" si="0"/>
         <v>0.94417903931916869</v>
       </c>
@@ -2207,7 +2094,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="57">
+      <c r="C5" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2215,87 +2102,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="58">
-        <f>Commercial!$C$21*outputfrac_elec</f>
-        <v>1.1817324639815762E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="58">
-        <f>Commercial!$C$21*outputfrac_coal</f>
-        <v>1.6681065025235112E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="58">
-        <f>Commercial!$C$21*outputfrac_ngps</f>
-        <v>3.7718097726775229E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="58">
-        <f>Commercial!$C$21*outputfrac_bio</f>
-        <v>5.196292126620005E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="57">
-        <f>Commercial!$C$21*outputfrac_other</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>